<commit_message>
This is issue1 commit
</commit_message>
<xml_diff>
--- a/firstexcel.xlsx
+++ b/firstexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Git Tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082D3FB-F5BD-45CA-8C0A-8B702F08B5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6304341-6A06-4D1B-AA2D-C8E59D73E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>S.No</t>
   </si>
@@ -33,19 +33,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Kiran</t>
   </si>
   <si>
-    <t>Nellore</t>
-  </si>
-  <si>
     <t>Prakash</t>
   </si>
   <si>
-    <t>Tadipatri</t>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -106,7 +103,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2CD134A6-58EA-4BCD-8F84-60CD1C114A13}" name="S.No"/>
     <tableColumn id="2" xr3:uid="{B7812FD6-2A55-4E47-BDAC-BFF35CC0506C}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{4FACDF9E-A859-4C07-9235-6E5DB8210D03}" name="City"/>
+    <tableColumn id="3" xr3:uid="{4FACDF9E-A859-4C07-9235-6E5DB8210D03}" name="Country"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -378,7 +375,7 @@
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,7 +391,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
@@ -402,10 +399,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -413,10 +410,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is master second commit
</commit_message>
<xml_diff>
--- a/firstexcel.xlsx
+++ b/firstexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Git Tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082D3FB-F5BD-45CA-8C0A-8B702F08B5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BD9204-DFDB-44E3-9C8E-5758F2127C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>S.No</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Tadipatri</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -101,12 +107,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1078590B-3B0D-4228-B55C-C8247A1B1025}" name="Table1" displayName="Table1" ref="B3:D7" totalsRowShown="0">
-  <autoFilter ref="B3:D7" xr:uid="{1078590B-3B0D-4228-B55C-C8247A1B1025}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1078590B-3B0D-4228-B55C-C8247A1B1025}" name="Table1" displayName="Table1" ref="B3:E7" totalsRowShown="0">
+  <autoFilter ref="B3:E7" xr:uid="{1078590B-3B0D-4228-B55C-C8247A1B1025}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2CD134A6-58EA-4BCD-8F84-60CD1C114A13}" name="S.No"/>
     <tableColumn id="2" xr3:uid="{B7812FD6-2A55-4E47-BDAC-BFF35CC0506C}" name="Name"/>
     <tableColumn id="3" xr3:uid="{4FACDF9E-A859-4C07-9235-6E5DB8210D03}" name="City"/>
+    <tableColumn id="4" xr3:uid="{B9BC0B77-681D-4E74-A038-7D14DA486CAF}" name="Country"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -375,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B3:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -386,7 +393,7 @@
     <col min="2" max="4" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -396,8 +403,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -407,8 +417,11 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -417,6 +430,9 @@
       </c>
       <c r="D5" t="s">
         <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>